<commit_message>
Some issues are fixed and new valid words are added to the tests
</commit_message>
<xml_diff>
--- a/Nuve/Resources/Tr/suffixes.xlsx
+++ b/Nuve/Resources/Tr/suffixes.xlsx
@@ -1816,9 +1816,6 @@
     <t>_mı, _mi, _mu, _mü</t>
   </si>
   <si>
-    <t>L_KESME_KALDIR, D_KESME_EKLE</t>
-  </si>
-  <si>
     <t>la, le, lı, li, lu, lü</t>
   </si>
   <si>
@@ -2828,6 +2825,9 @@
   </si>
   <si>
     <t xml:space="preserve">DONUSUM_U, YUMUSAMA_kğ, </t>
+  </si>
+  <si>
+    <t>KESME_KALDIR, KESME_EKLE</t>
   </si>
 </sst>
 </file>
@@ -3159,9 +3159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Ofis">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3199,7 +3199,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Ofis">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3271,7 +3271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Ofis">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3448,10 +3448,10 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H102" sqref="H102"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3482,7 +3482,7 @@
         <v>267</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>268</v>
@@ -3503,7 +3503,7 @@
         <v>270</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>274</v>
@@ -3538,7 +3538,7 @@
         <v>281</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>193</v>
@@ -3579,10 +3579,10 @@
         <v>319</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>317</v>
@@ -3591,7 +3591,7 @@
         <v>318</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>320</v>
@@ -3620,10 +3620,10 @@
         <v>319</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>331</v>
@@ -3632,7 +3632,7 @@
         <v>332</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>333</v>
@@ -3661,10 +3661,10 @@
         <v>319</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>325</v>
@@ -3673,7 +3673,7 @@
         <v>326</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>327</v>
@@ -3702,10 +3702,10 @@
         <v>319</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>322</v>
@@ -3714,7 +3714,7 @@
         <v>323</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>324</v>
@@ -3740,10 +3740,10 @@
         <v>319</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>334</v>
@@ -3752,7 +3752,7 @@
         <v>335</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>336</v>
@@ -3778,7 +3778,7 @@
         <v>319</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>194</v>
@@ -3790,7 +3790,7 @@
         <v>330</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -3813,10 +3813,10 @@
         <v>293</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>313</v>
@@ -3825,7 +3825,7 @@
         <v>314</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3848,7 +3848,7 @@
         <v>293</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>196</v>
@@ -3883,10 +3883,10 @@
         <v>293</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>299</v>
@@ -3895,7 +3895,7 @@
         <v>300</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>301</v>
@@ -3921,7 +3921,7 @@
         <v>293</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>197</v>
@@ -3930,7 +3930,7 @@
         <v>297</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>298</v>
@@ -3956,10 +3956,10 @@
         <v>293</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>302</v>
@@ -3968,7 +3968,7 @@
         <v>303</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -3991,7 +3991,7 @@
         <v>293</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>198</v>
@@ -4026,10 +4026,10 @@
         <v>293</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>291</v>
@@ -4038,7 +4038,7 @@
         <v>292</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -4061,7 +4061,7 @@
         <v>293</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>199</v>
@@ -4096,10 +4096,10 @@
         <v>293</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>307</v>
@@ -4108,7 +4108,7 @@
         <v>308</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>309</v>
@@ -4134,7 +4134,7 @@
         <v>293</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>200</v>
@@ -4146,7 +4146,7 @@
         <v>311</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>312</v>
@@ -4169,7 +4169,7 @@
         <v>281</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>592</v>
@@ -4227,7 +4227,7 @@
         <v>281</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>193</v>
@@ -4256,10 +4256,10 @@
         <v>569</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>599</v>
+        <v>723</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>569</v>
@@ -4277,7 +4277,7 @@
         <v>588</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>588</v>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
@@ -4304,7 +4304,7 @@
         <v>281</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>191</v>
@@ -4359,7 +4359,7 @@
         <v>281</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>193</v>
@@ -4391,7 +4391,7 @@
         <v>364</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>201</v>
@@ -4403,7 +4403,7 @@
         <v>363</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>365</v>
@@ -4432,7 +4432,7 @@
         <v>349</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>202</v>
@@ -4441,7 +4441,7 @@
         <v>348</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -4464,7 +4464,7 @@
         <v>349</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>203</v>
@@ -4473,7 +4473,7 @@
         <v>355</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -4496,7 +4496,7 @@
         <v>349</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>204</v>
@@ -4505,7 +4505,7 @@
         <v>351</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -4528,7 +4528,7 @@
         <v>349</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>205</v>
@@ -4537,7 +4537,7 @@
         <v>357</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -4560,7 +4560,7 @@
         <v>349</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>193</v>
@@ -4650,7 +4650,7 @@
         <v>349</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>208</v>
@@ -4682,7 +4682,7 @@
         <v>349</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>209</v>
@@ -4714,7 +4714,7 @@
         <v>343</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>210</v>
@@ -4752,7 +4752,7 @@
         <v>343</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>211</v>
@@ -4764,7 +4764,7 @@
         <v>360</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>361</v>
@@ -4790,7 +4790,7 @@
         <v>343</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>273</v>
@@ -4802,7 +4802,7 @@
         <v>346</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>347</v>
@@ -4828,7 +4828,7 @@
         <v>343</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>272</v>
@@ -4840,7 +4840,7 @@
         <v>341</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>344</v>
@@ -4866,7 +4866,7 @@
         <v>373</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>212</v>
@@ -4898,7 +4898,7 @@
         <v>373</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>213</v>
@@ -4930,7 +4930,7 @@
         <v>373</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>203</v>
@@ -4962,7 +4962,7 @@
         <v>373</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>214</v>
@@ -4994,7 +4994,7 @@
         <v>373</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>215</v>
@@ -5029,7 +5029,7 @@
         <v>373</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>216</v>
@@ -5061,7 +5061,7 @@
         <v>373</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>217</v>
@@ -5093,7 +5093,7 @@
         <v>373</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>218</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>79</v>
@@ -5128,7 +5128,7 @@
         <v>373</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>219</v>
@@ -5163,7 +5163,7 @@
         <v>396</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>220</v>
@@ -5175,7 +5175,7 @@
         <v>395</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="O50" s="1" t="s">
         <v>397</v>
@@ -5201,7 +5201,7 @@
         <v>396</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>221</v>
@@ -5213,7 +5213,7 @@
         <v>399</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>400</v>
@@ -5239,7 +5239,7 @@
         <v>396</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>222</v>
@@ -5251,7 +5251,7 @@
         <v>402</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -5274,7 +5274,7 @@
         <v>396</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>223</v>
@@ -5286,7 +5286,7 @@
         <v>406</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>407</v>
@@ -5315,13 +5315,13 @@
         <v>396</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>224</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>403</v>
@@ -5330,7 +5330,7 @@
         <v>404</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>561</v>
@@ -5356,7 +5356,7 @@
         <v>412</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>225</v>
@@ -5368,7 +5368,7 @@
         <v>410</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>413</v>
@@ -5394,7 +5394,7 @@
         <v>412</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>226</v>
@@ -5406,7 +5406,7 @@
         <v>415</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="O56" s="1" t="s">
         <v>416</v>
@@ -5432,7 +5432,7 @@
         <v>412</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>227</v>
@@ -5444,7 +5444,7 @@
         <v>418</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="O57" s="1" t="s">
         <v>419</v>
@@ -5470,7 +5470,7 @@
         <v>412</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>228</v>
@@ -5482,7 +5482,7 @@
         <v>421</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="O58" s="1" t="s">
         <v>422</v>
@@ -5508,7 +5508,7 @@
         <v>424</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>229</v>
@@ -5546,7 +5546,7 @@
         <v>576</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>230</v>
@@ -5558,7 +5558,7 @@
         <v>428</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>430</v>
@@ -5584,7 +5584,7 @@
         <v>424</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>231</v>
@@ -5596,7 +5596,7 @@
         <v>432</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="O61" s="1" t="s">
         <v>433</v>
@@ -5622,7 +5622,7 @@
         <v>424</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>232</v>
@@ -5634,7 +5634,7 @@
         <v>435</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="O62" s="1" t="s">
         <v>436</v>
@@ -5657,7 +5657,7 @@
         <v>438</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>233</v>
@@ -5669,7 +5669,7 @@
         <v>437</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -5689,7 +5689,7 @@
         <v>438</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>234</v>
@@ -5721,7 +5721,7 @@
         <v>438</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>235</v>
@@ -5733,7 +5733,7 @@
         <v>443</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
@@ -5753,7 +5753,7 @@
         <v>446</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>222</v>
@@ -5765,7 +5765,7 @@
         <v>445</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
@@ -5785,7 +5785,7 @@
         <v>446</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>236</v>
@@ -5817,7 +5817,7 @@
         <v>446</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>237</v>
@@ -5846,7 +5846,7 @@
         <v>446</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>238</v>
@@ -5875,7 +5875,7 @@
         <v>446</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>591</v>
@@ -5901,7 +5901,7 @@
         <v>446</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>239</v>
@@ -5933,7 +5933,7 @@
         <v>446</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>221</v>
@@ -5945,7 +5945,7 @@
         <v>459</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
@@ -5965,7 +5965,7 @@
         <v>460</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>195</v>
@@ -5994,7 +5994,7 @@
         <v>460</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>240</v>
@@ -6020,7 +6020,7 @@
         <v>460</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>241</v>
@@ -6032,7 +6032,7 @@
         <v>465</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>466</v>
@@ -6055,7 +6055,7 @@
         <v>460</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>242</v>
@@ -6084,7 +6084,7 @@
         <v>460</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>243</v>
@@ -6093,7 +6093,7 @@
         <v>469</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="O77" s="1" t="s">
         <v>470</v>
@@ -6116,7 +6116,7 @@
         <v>460</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>244</v>
@@ -6145,7 +6145,7 @@
         <v>460</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>245</v>
@@ -6154,7 +6154,7 @@
         <v>473</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>474</v>
@@ -6177,7 +6177,7 @@
         <v>460</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>246</v>
@@ -6189,7 +6189,7 @@
         <v>476</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="O80" s="1" t="s">
         <v>477</v>
@@ -6212,7 +6212,7 @@
         <v>460</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>247</v>
@@ -6241,7 +6241,7 @@
         <v>460</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>248</v>
@@ -6270,7 +6270,7 @@
         <v>411</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>249</v>
@@ -6305,7 +6305,7 @@
         <v>438</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>250</v>
@@ -6334,7 +6334,7 @@
         <v>438</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>251</v>
@@ -6346,7 +6346,7 @@
         <v>511</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="O85" s="1" t="s">
         <v>512</v>
@@ -6369,7 +6369,7 @@
         <v>411</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>252</v>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>52</v>
@@ -6421,7 +6421,7 @@
         <v>411</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>572</v>
@@ -6433,7 +6433,7 @@
         <v>490</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="N88" s="1" t="s">
         <v>491</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>39</v>
@@ -6453,10 +6453,10 @@
         <v>108</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O89" s="1" t="s">
         <v>496</v>
@@ -6464,7 +6464,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>153</v>
@@ -6473,15 +6473,15 @@
         <v>108</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>39</v>
@@ -6496,7 +6496,7 @@
         <v>411</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>574</v>
@@ -6508,13 +6508,13 @@
         <v>494</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>495</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -6534,7 +6534,7 @@
         <v>411</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>255</v>
@@ -6546,7 +6546,7 @@
         <v>505</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N92" s="1" t="s">
         <v>487</v>
@@ -6598,7 +6598,7 @@
         <v>411</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>574</v>
@@ -6633,7 +6633,7 @@
         <v>411</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>254</v>
@@ -6645,7 +6645,7 @@
         <v>501</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N95" s="1" t="s">
         <v>502</v>
@@ -6671,10 +6671,10 @@
         <v>515</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>513</v>
@@ -6683,7 +6683,7 @@
         <v>514</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N96" s="1" t="s">
         <v>570</v>
@@ -6706,7 +6706,7 @@
         <v>515</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>256</v>
@@ -6738,10 +6738,10 @@
         <v>521</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>519</v>
@@ -6770,7 +6770,7 @@
         <v>521</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>257</v>
@@ -6782,7 +6782,7 @@
         <v>524</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
@@ -6802,7 +6802,7 @@
         <v>521</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>258</v>
@@ -6814,7 +6814,7 @@
         <v>526</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
@@ -6834,10 +6834,10 @@
         <v>521</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>527</v>
@@ -6846,7 +6846,7 @@
         <v>528</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
@@ -6866,7 +6866,7 @@
         <v>531</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>259</v>
@@ -6878,7 +6878,7 @@
         <v>530</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
@@ -6898,10 +6898,10 @@
         <v>531</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>532</v>
@@ -6930,7 +6930,7 @@
         <v>531</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>260</v>
@@ -6962,7 +6962,7 @@
         <v>531</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>261</v>
@@ -6974,7 +6974,7 @@
         <v>539</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
@@ -6994,10 +6994,10 @@
         <v>531</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>540</v>
@@ -7006,7 +7006,7 @@
         <v>541</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
@@ -7023,7 +7023,7 @@
         <v>108</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>262</v>
@@ -7046,10 +7046,10 @@
         <v>544</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>542</v>
@@ -7058,7 +7058,7 @@
         <v>543</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
@@ -7078,7 +7078,7 @@
         <v>544</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>245</v>
@@ -7107,7 +7107,7 @@
         <v>555</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>578</v>
@@ -7142,7 +7142,7 @@
         <v>559</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>263</v>
@@ -7171,7 +7171,7 @@
         <v>548</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>264</v>
@@ -7183,7 +7183,7 @@
         <v>547</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O112" s="1" t="s">
         <v>549</v>
@@ -7206,7 +7206,7 @@
         <v>548</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>265</v>
@@ -7238,7 +7238,7 @@
         <v>581</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>598</v>
@@ -7267,7 +7267,7 @@
         <v>581</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>595</v>

</xml_diff>

<commit_message>
the suffixes comes after space character are supported now
</commit_message>
<xml_diff>
--- a/Nuve/Resources/Tr/suffixes.xlsx
+++ b/Nuve/Resources/Tr/suffixes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="930" windowWidth="15240" windowHeight="8070" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="930" windowWidth="15240" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="suffix" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="738">
   <si>
     <t>Un</t>
   </si>
@@ -1779,9 +1779,6 @@
   </si>
   <si>
     <t xml:space="preserve">DONUSUM_C, DONUSUM_A, </t>
-  </si>
-  <si>
-    <t>DONUSUM_U</t>
   </si>
   <si>
     <t>DONUSUM_U, DUSME_UNSUZ, OZEL_N</t>
@@ -2824,6 +2821,12 @@
   </si>
   <si>
     <t>Short Description</t>
+  </si>
+  <si>
+    <t>DONUSUM_U, ALTTIRE_KALDIR</t>
+  </si>
+  <si>
+    <t>DONUSUM_A, ALTTIRE_KALDIR</t>
   </si>
 </sst>
 </file>
@@ -3235,9 +3238,9 @@
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id" dataDxfId="4"/>
-    <tableColumn id="11" name="Short Description" dataDxfId="1"/>
-    <tableColumn id="9" name="surfaces" dataDxfId="3"/>
-    <tableColumn id="12" name="Örnekler" dataDxfId="2"/>
+    <tableColumn id="11" name="Short Description" dataDxfId="3"/>
+    <tableColumn id="9" name="surfaces" dataDxfId="2"/>
+    <tableColumn id="12" name="Örnekler" dataDxfId="1"/>
     <tableColumn id="10" name="Zemberek Karşılığı" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3533,11 +3536,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3547,9 +3550,9 @@
     <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="62.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -3677,7 +3680,7 @@
         <v>282</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>284</v>
@@ -3718,7 +3721,7 @@
         <v>296</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>297</v>
@@ -3747,7 +3750,7 @@
         <v>283</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>556</v>
@@ -3759,7 +3762,7 @@
         <v>290</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>291</v>
@@ -3800,7 +3803,7 @@
         <v>287</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>288</v>
@@ -3838,7 +3841,7 @@
         <v>299</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>300</v>
@@ -3864,7 +3867,7 @@
         <v>283</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>177</v>
@@ -3876,7 +3879,7 @@
         <v>294</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -3911,7 +3914,7 @@
         <v>280</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3922,7 +3925,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>524</v>
@@ -3946,7 +3949,7 @@
         <v>269</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>270</v>
@@ -3984,7 +3987,7 @@
         <v>272</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -4019,7 +4022,7 @@
         <v>266</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -4054,7 +4057,7 @@
         <v>274</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>275</v>
@@ -4092,7 +4095,7 @@
         <v>277</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>278</v>
@@ -4115,7 +4118,7 @@
         <v>255</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>532</v>
@@ -4144,7 +4147,7 @@
         <v>551</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>515</v>
@@ -4215,7 +4218,7 @@
         <v>324</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>326</v>
@@ -4253,7 +4256,7 @@
         <v>309</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -4285,7 +4288,7 @@
         <v>316</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -4317,7 +4320,7 @@
         <v>312</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -4349,7 +4352,7 @@
         <v>318</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -4462,7 +4465,7 @@
         <v>310</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>187</v>
@@ -4576,7 +4579,7 @@
         <v>321</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>322</v>
@@ -4614,7 +4617,7 @@
         <v>307</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>308</v>
@@ -4652,7 +4655,7 @@
         <v>302</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>305</v>
@@ -4987,7 +4990,7 @@
         <v>356</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>358</v>
@@ -5025,7 +5028,7 @@
         <v>360</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>361</v>
@@ -5051,7 +5054,7 @@
         <v>357</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>201</v>
@@ -5063,7 +5066,7 @@
         <v>363</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -5086,7 +5089,7 @@
         <v>357</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>202</v>
@@ -5098,7 +5101,7 @@
         <v>367</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>368</v>
@@ -5127,7 +5130,7 @@
         <v>357</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>203</v>
@@ -5142,7 +5145,7 @@
         <v>365</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>510</v>
@@ -5180,7 +5183,7 @@
         <v>371</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>374</v>
@@ -5218,7 +5221,7 @@
         <v>376</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="O47" s="1" t="s">
         <v>377</v>
@@ -5256,7 +5259,7 @@
         <v>379</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>380</v>
@@ -5294,7 +5297,7 @@
         <v>382</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O49" s="1" t="s">
         <v>383</v>
@@ -5370,7 +5373,7 @@
         <v>389</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>391</v>
@@ -5408,7 +5411,7 @@
         <v>393</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>394</v>
@@ -5446,7 +5449,7 @@
         <v>396</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>397</v>
@@ -5481,7 +5484,7 @@
         <v>398</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
@@ -5545,7 +5548,7 @@
         <v>404</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
@@ -5565,7 +5568,7 @@
         <v>407</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>201</v>
@@ -5577,7 +5580,7 @@
         <v>406</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -5687,7 +5690,7 @@
         <v>407</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>531</v>
@@ -5757,7 +5760,7 @@
         <v>420</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -5844,7 +5847,7 @@
         <v>426</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>427</v>
@@ -5905,7 +5908,7 @@
         <v>430</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O68" s="1" t="s">
         <v>431</v>
@@ -5966,7 +5969,7 @@
         <v>434</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>435</v>
@@ -6001,7 +6004,7 @@
         <v>437</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>438</v>
@@ -6158,7 +6161,7 @@
         <v>460</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="O76" s="1" t="s">
         <v>461</v>
@@ -6233,7 +6236,7 @@
         <v>372</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>518</v>
@@ -6245,7 +6248,7 @@
         <v>451</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>452</v>
@@ -6265,7 +6268,7 @@
         <v>99</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>540</v>
@@ -6285,7 +6288,7 @@
         <v>99</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>541</v>
@@ -6320,7 +6323,7 @@
         <v>463</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>516</v>
@@ -6419,7 +6422,7 @@
         <v>473</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
@@ -6439,7 +6442,7 @@
         <v>470</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>234</v>
@@ -6451,7 +6454,7 @@
         <v>475</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
@@ -6471,7 +6474,7 @@
         <v>470</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>548</v>
@@ -6483,7 +6486,7 @@
         <v>477</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
@@ -6515,7 +6518,7 @@
         <v>479</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
@@ -6611,7 +6614,7 @@
         <v>488</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -6643,7 +6646,7 @@
         <v>490</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
@@ -6675,7 +6678,7 @@
         <v>492</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
@@ -6800,7 +6803,7 @@
         <v>496</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="O97" s="1" t="s">
         <v>498</v>
@@ -6855,7 +6858,7 @@
         <v>524</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>587</v>
+        <v>736</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>536</v>
@@ -6884,7 +6887,7 @@
         <v>524</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>563</v>
+        <v>737</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>533</v>
@@ -6903,7 +6906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
@@ -6922,7 +6925,7 @@
         <v>241</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>245</v>
@@ -6939,7 +6942,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>176</v>
@@ -6956,13 +6959,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>554</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>281</v>
@@ -6973,13 +6976,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>555</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>295</v>
@@ -6990,13 +6993,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>556</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>289</v>
@@ -7007,13 +7010,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>557</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>286</v>
@@ -7024,13 +7027,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>558</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>298</v>
@@ -7041,13 +7044,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>177</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>293</v>
@@ -7058,13 +7061,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>562</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>279</v>
@@ -7075,13 +7078,13 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>561</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>268</v>
@@ -7092,13 +7095,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>560</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>271</v>
@@ -7109,13 +7112,13 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>559</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>265</v>
@@ -7126,13 +7129,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>544</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>273</v>
@@ -7143,13 +7146,13 @@
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>179</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>276</v>
@@ -7160,7 +7163,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>532</v>
@@ -7177,7 +7180,7 @@
         <v>528</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>515</v>
@@ -7190,7 +7193,7 @@
         <v>511</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>176</v>
@@ -7203,13 +7206,13 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>180</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>323</v>
@@ -7220,13 +7223,13 @@
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>181</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>309</v>
@@ -7237,13 +7240,13 @@
         <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>182</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>316</v>
@@ -7254,13 +7257,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>183</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>312</v>
@@ -7271,13 +7274,13 @@
         <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>184</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>318</v>
@@ -7288,7 +7291,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>176</v>
@@ -7305,7 +7308,7 @@
         <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>185</v>
@@ -7322,7 +7325,7 @@
         <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>186</v>
@@ -7339,7 +7342,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>187</v>
@@ -7356,7 +7359,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>188</v>
@@ -7390,13 +7393,13 @@
         <v>50</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>190</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>320</v>
@@ -7407,13 +7410,13 @@
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>247</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>306</v>
@@ -7424,13 +7427,13 @@
         <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>246</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>301</v>
@@ -7441,7 +7444,7 @@
         <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>191</v>
@@ -7458,7 +7461,7 @@
         <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>192</v>
@@ -7475,7 +7478,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>182</v>
@@ -7492,7 +7495,7 @@
         <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>193</v>
@@ -7509,7 +7512,7 @@
         <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>194</v>
@@ -7526,7 +7529,7 @@
         <v>64</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>195</v>
@@ -7543,7 +7546,7 @@
         <v>66</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>196</v>
@@ -7560,7 +7563,7 @@
         <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>197</v>
@@ -7577,7 +7580,7 @@
         <v>545</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>198</v>
@@ -7594,13 +7597,13 @@
         <v>71</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>199</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>355</v>
@@ -7611,13 +7614,13 @@
         <v>73</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>200</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>359</v>
@@ -7628,13 +7631,13 @@
         <v>75</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>201</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>362</v>
@@ -7645,13 +7648,13 @@
         <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>202</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>366</v>
@@ -7662,13 +7665,13 @@
         <v>79</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>203</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>364</v>
@@ -7679,13 +7682,13 @@
         <v>81</v>
       </c>
       <c r="B46" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>204</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>370</v>
@@ -7696,13 +7699,13 @@
         <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>205</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>375</v>
@@ -7713,13 +7716,13 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>206</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>378</v>
@@ -7730,13 +7733,13 @@
         <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>207</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>381</v>
@@ -7747,7 +7750,7 @@
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>208</v>
@@ -7764,13 +7767,13 @@
         <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>209</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>388</v>
@@ -7781,13 +7784,13 @@
         <v>93</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>210</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>392</v>
@@ -7798,13 +7801,13 @@
         <v>95</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>211</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>395</v>
@@ -7815,13 +7818,13 @@
         <v>97</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>212</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>530</v>
@@ -7832,7 +7835,7 @@
         <v>100</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>213</v>
@@ -7849,13 +7852,13 @@
         <v>102</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>214</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>403</v>
@@ -7866,13 +7869,13 @@
         <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>201</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>405</v>
@@ -7883,7 +7886,7 @@
         <v>105</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>215</v>
@@ -7900,7 +7903,7 @@
         <v>107</v>
       </c>
       <c r="B59" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>216</v>
@@ -7917,7 +7920,7 @@
         <v>109</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>217</v>
@@ -7934,7 +7937,7 @@
         <v>111</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>531</v>
@@ -7949,7 +7952,7 @@
         <v>113</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>218</v>
@@ -7966,13 +7969,13 @@
         <v>115</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>200</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>419</v>
@@ -7983,7 +7986,7 @@
         <v>116</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>178</v>
@@ -7998,7 +8001,7 @@
         <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>219</v>
@@ -8013,13 +8016,13 @@
         <v>119</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>220</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>425</v>
@@ -8030,7 +8033,7 @@
         <v>121</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>221</v>
@@ -8047,13 +8050,13 @@
         <v>123</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>222</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>430</v>
@@ -8064,7 +8067,7 @@
         <v>125</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>223</v>
@@ -8081,13 +8084,13 @@
         <v>127</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>434</v>
@@ -8098,13 +8101,13 @@
         <v>129</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>225</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>436</v>
@@ -8115,7 +8118,7 @@
         <v>131</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>226</v>
@@ -8132,7 +8135,7 @@
         <v>133</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>227</v>
@@ -8149,7 +8152,7 @@
         <v>135</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>228</v>
@@ -8166,7 +8169,7 @@
         <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>229</v>
@@ -8181,13 +8184,13 @@
         <v>139</v>
       </c>
       <c r="B76" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>230</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>459</v>
@@ -8198,7 +8201,7 @@
         <v>141</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>231</v>
@@ -8215,7 +8218,7 @@
         <v>542</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>43</v>
@@ -8228,13 +8231,13 @@
         <v>517</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>518</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>450</v>
@@ -8245,7 +8248,7 @@
         <v>538</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>540</v>
@@ -8258,7 +8261,7 @@
         <v>539</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>541</v>
@@ -8274,7 +8277,7 @@
         <v>537</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>462</v>
@@ -8285,7 +8288,7 @@
         <v>146</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>232</v>
@@ -8302,7 +8305,7 @@
         <v>148</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>549</v>
@@ -8319,13 +8322,13 @@
         <v>150</v>
       </c>
       <c r="B85" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>233</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>472</v>
@@ -8336,13 +8339,13 @@
         <v>152</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>234</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>474</v>
@@ -8353,13 +8356,13 @@
         <v>154</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>548</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>476</v>
@@ -8370,13 +8373,13 @@
         <v>156</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>235</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>478</v>
@@ -8387,7 +8390,7 @@
         <v>158</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>546</v>
@@ -8404,7 +8407,7 @@
         <v>160</v>
       </c>
       <c r="B90" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>236</v>
@@ -8421,13 +8424,13 @@
         <v>162</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>237</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>487</v>
@@ -8438,13 +8441,13 @@
         <v>163</v>
       </c>
       <c r="B92" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>547</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>489</v>
@@ -8455,13 +8458,13 @@
         <v>165</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>543</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>491</v>
@@ -8472,7 +8475,7 @@
         <v>167</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>224</v>
@@ -8489,7 +8492,7 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>521</v>
@@ -8506,7 +8509,7 @@
         <v>170</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>238</v>
@@ -8523,13 +8526,13 @@
         <v>172</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>239</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>495</v>
@@ -8540,7 +8543,7 @@
         <v>174</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>240</v>
@@ -8557,7 +8560,7 @@
         <v>523</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>536</v>
@@ -8574,7 +8577,7 @@
         <v>529</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>533</v>

</xml_diff>

<commit_message>
Suffixes with empty surfaces are now supported
</commit_message>
<xml_diff>
--- a/Nuve/Resources/Tr/suffixes.xlsx
+++ b/Nuve/Resources/Tr/suffixes.xlsx
@@ -11,14 +11,14 @@
     <sheet name="desc" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">suffix!$A$1:$O$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">suffix!$A$1:$O$99</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="739">
   <si>
     <t>Un</t>
   </si>
@@ -2827,6 +2827,9 @@
   </si>
   <si>
     <t>DONUSUM_A, ALTTIRE_KALDIR</t>
+  </si>
+  <si>
+    <t>FC_KIP_EMIR_0</t>
   </si>
 </sst>
 </file>
@@ -3210,8 +3213,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O100" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:O100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O101" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:O101"/>
   <tableColumns count="15">
     <tableColumn id="1" name="id" dataDxfId="21"/>
     <tableColumn id="2" name="lexicalForm" dataDxfId="20"/>
@@ -3534,13 +3537,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4663,42 +4666,37 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E32" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>335</v>
-      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
@@ -4716,21 +4714,21 @@
         <v>566</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>1</v>
@@ -4745,24 +4743,24 @@
         <v>334</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>1</v>
@@ -4777,24 +4775,24 @@
         <v>334</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>1</v>
@@ -4809,27 +4807,24 @@
         <v>334</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
@@ -4844,24 +4839,27 @@
         <v>334</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>346</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>1</v>
@@ -4876,24 +4874,24 @@
         <v>334</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
@@ -4911,24 +4909,21 @@
         <v>573</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>545</v>
+        <v>68</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>1</v>
@@ -4943,27 +4938,27 @@
         <v>334</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>545</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>1</v>
@@ -4975,33 +4970,30 @@
         <v>333</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>1</v>
@@ -5016,30 +5008,30 @@
         <v>357</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>1</v>
@@ -5054,27 +5046,30 @@
         <v>357</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>647</v>
+        <v>567</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>1</v>
@@ -5089,33 +5084,27 @@
         <v>357</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>369</v>
+        <v>614</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>1</v>
@@ -5130,71 +5119,74 @@
         <v>357</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>553</v>
+        <v>202</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>591</v>
+        <v>615</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>368</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>510</v>
+        <v>369</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>99</v>
+        <v>524</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>372</v>
+        <v>333</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>565</v>
+        <v>643</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>553</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>616</v>
+        <v>591</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>374</v>
+        <v>510</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>1</v>
@@ -5212,27 +5204,27 @@
         <v>565</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1</v>
@@ -5250,27 +5242,27 @@
         <v>565</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>1</v>
@@ -5288,27 +5280,27 @@
         <v>565</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1</v>
@@ -5320,30 +5312,33 @@
         <v>372</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>382</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>386</v>
+        <v>619</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>1</v>
@@ -5355,36 +5350,30 @@
         <v>372</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>519</v>
+        <v>385</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>620</v>
+        <v>386</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>1</v>
@@ -5396,33 +5385,36 @@
         <v>372</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>385</v>
+        <v>390</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>1</v>
@@ -5440,59 +5432,65 @@
         <v>565</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>399</v>
+        <v>372</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>385</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>530</v>
+        <v>395</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>99</v>
@@ -5504,27 +5502,27 @@
         <v>399</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>400</v>
+        <v>530</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>402</v>
+        <v>623</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>99</v>
@@ -5539,24 +5537,24 @@
         <v>563</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>624</v>
+        <v>402</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>99</v>
@@ -5565,30 +5563,30 @@
         <v>99</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>647</v>
+        <v>563</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>99</v>
@@ -5600,27 +5598,27 @@
         <v>407</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>575</v>
+        <v>647</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>410</v>
+        <v>625</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>99</v>
@@ -5632,24 +5630,27 @@
         <v>407</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>99</v>
@@ -5664,21 +5665,21 @@
         <v>576</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>99</v>
@@ -5690,21 +5691,24 @@
         <v>407</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>648</v>
+        <v>576</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>531</v>
+        <v>217</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>99</v>
@@ -5716,27 +5720,21 @@
         <v>407</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>563</v>
+        <v>648</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>218</v>
+        <v>531</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>99</v>
@@ -5748,27 +5746,27 @@
         <v>407</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>626</v>
+        <v>418</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>99</v>
@@ -5777,27 +5775,30 @@
         <v>99</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>178</v>
+        <v>200</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>420</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="O64" s="1" t="s">
-        <v>423</v>
+        <v>626</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>99</v>
@@ -5809,21 +5810,24 @@
         <v>421</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>99</v>
@@ -5835,30 +5839,21 @@
         <v>421</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>426</v>
+        <v>219</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="N66" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>99</v>
@@ -5870,24 +5865,30 @@
         <v>421</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>426</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>429</v>
+        <v>627</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>99</v>
@@ -5899,27 +5900,24 @@
         <v>421</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="O68" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>99</v>
@@ -5931,24 +5929,27 @@
         <v>421</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>433</v>
+        <v>628</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>99</v>
@@ -5960,27 +5961,24 @@
         <v>421</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="N70" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>99</v>
@@ -5992,30 +5990,27 @@
         <v>421</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="O71" s="1" t="s">
-        <v>438</v>
+        <v>629</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>99</v>
@@ -6027,24 +6022,30 @@
         <v>421</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>440</v>
+        <v>630</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>99</v>
@@ -6056,88 +6057,88 @@
         <v>421</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>581</v>
+        <v>563</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>372</v>
+        <v>421</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>563</v>
+        <v>581</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>563</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>456</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="N75" s="1" t="s">
-        <v>444</v>
+        <v>457</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>99</v>
@@ -6149,30 +6150,24 @@
         <v>399</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>460</v>
+        <v>229</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="O76" s="1" t="s">
-        <v>461</v>
+        <v>443</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>99</v>
@@ -6181,160 +6176,160 @@
         <v>99</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>372</v>
+        <v>399</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="N77" s="1" t="s">
-        <v>448</v>
+        <v>631</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>542</v>
+        <v>141</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="E78" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>583</v>
+      </c>
       <c r="I78" s="1" t="s">
-        <v>43</v>
+        <v>231</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>644</v>
-      </c>
       <c r="I79" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="M79" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="N79" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="O79" s="1" t="s">
-        <v>453</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>30</v>
+        <v>142</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="E80" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="H80" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>540</v>
+        <v>518</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>143</v>
+        <v>30</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>144</v>
+        <v>539</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>464</v>
-      </c>
       <c r="H82" s="1" t="s">
-        <v>563</v>
+        <v>646</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="K82" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="L82" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="M82" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="N82" s="1" t="s">
-        <v>516</v>
+        <v>541</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>99</v>
@@ -6349,24 +6344,27 @@
         <v>563</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>232</v>
+        <v>537</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>467</v>
+        <v>633</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>99</v>
@@ -6375,30 +6373,30 @@
         <v>99</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>549</v>
+        <v>232</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>99</v>
@@ -6410,27 +6408,27 @@
         <v>470</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>233</v>
+        <v>549</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>634</v>
+        <v>471</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>99</v>
@@ -6442,27 +6440,27 @@
         <v>470</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>649</v>
+        <v>584</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>99</v>
@@ -6474,27 +6472,27 @@
         <v>470</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>548</v>
+        <v>234</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>99</v>
@@ -6503,30 +6501,30 @@
         <v>99</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>583</v>
+        <v>650</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>235</v>
+        <v>548</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>99</v>
@@ -6538,27 +6536,27 @@
         <v>480</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>546</v>
+        <v>235</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>483</v>
+        <v>637</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>99</v>
@@ -6570,27 +6568,27 @@
         <v>480</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>236</v>
+        <v>546</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>99</v>
@@ -6602,30 +6600,30 @@
         <v>480</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>585</v>
+        <v>563</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>638</v>
+        <v>486</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>164</v>
+        <v>8</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>99</v>
@@ -6634,27 +6632,27 @@
         <v>480</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>567</v>
+        <v>585</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>547</v>
+        <v>237</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>1</v>
@@ -6663,33 +6661,33 @@
         <v>99</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>586</v>
+        <v>567</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>99</v>
@@ -6698,24 +6696,27 @@
         <v>493</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>224</v>
+        <v>543</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>434</v>
+        <v>491</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>494</v>
+        <v>640</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>99</v>
@@ -6724,33 +6725,27 @@
         <v>99</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>563</v>
+        <v>579</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>521</v>
+        <v>224</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="L95" s="1" t="s">
-        <v>503</v>
+        <v>434</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="O95" s="1" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>99</v>
@@ -6759,27 +6754,33 @@
         <v>99</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>238</v>
+        <v>521</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>507</v>
+        <v>522</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>99</v>
@@ -6788,33 +6789,27 @@
         <v>99</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>583</v>
+        <v>567</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="L97" s="1" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="O97" s="1" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>99</v>
@@ -6826,59 +6821,65 @@
         <v>497</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>565</v>
+        <v>583</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>501</v>
+        <v>641</v>
       </c>
       <c r="O98" s="1" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>523</v>
+        <v>174</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>535</v>
+        <v>175</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>524</v>
+        <v>99</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>524</v>
+        <v>99</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>497</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>736</v>
+        <v>565</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>536</v>
+        <v>240</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>525</v>
+        <v>499</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>500</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="N99" s="1" t="s">
-        <v>527</v>
+        <v>501</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>524</v>
@@ -6887,9 +6888,38 @@
         <v>524</v>
       </c>
       <c r="H100" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="N100" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="H101" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="I100" s="1" t="s">
+      <c r="I101" s="1" t="s">
         <v>533</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for returning all solutions with empty transitions
</commit_message>
<xml_diff>
--- a/Nuve/Resources/Tr/suffixes.xlsx
+++ b/Nuve/Resources/Tr/suffixes.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="740">
   <si>
     <t>Un</t>
   </si>
@@ -2544,9 +2544,6 @@
     <t xml:space="preserve">OZEL_UYOR, DONUSUM_U, </t>
   </si>
   <si>
-    <t xml:space="preserve">OZEL_GZ, DUSME_UNLU_GZ, DONUSUM_U, DONUSUM_A, </t>
-  </si>
-  <si>
     <t xml:space="preserve">OZEL_EDILGEN, DUSME_UNLU, DONUSUM_U, </t>
   </si>
   <si>
@@ -2830,6 +2827,12 @@
   </si>
   <si>
     <t>FC_KIP_EMIR_0</t>
+  </si>
+  <si>
+    <t>yım, yim, yum, yüm, ım, im, um, üm, m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GZ_OLUMSUZ, OZEL_GZ, DUSME_UNLU_GZ, DONUSUM_U, DONUSUM_A, </t>
   </si>
 </sst>
 </file>
@@ -3540,10 +3543,10 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3928,7 +3931,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>524</v>
@@ -4150,7 +4153,7 @@
         <v>551</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>515</v>
@@ -4253,7 +4256,7 @@
         <v>566</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>181</v>
+        <v>738</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>309</v>
@@ -4666,7 +4669,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
@@ -5084,7 +5087,7 @@
         <v>357</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>201</v>
@@ -5160,7 +5163,7 @@
         <v>357</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>643</v>
+        <v>739</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>203</v>
@@ -5598,7 +5601,7 @@
         <v>407</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>201</v>
@@ -5720,7 +5723,7 @@
         <v>407</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>531</v>
@@ -6266,7 +6269,7 @@
         <v>372</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>518</v>
@@ -6298,7 +6301,7 @@
         <v>99</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>540</v>
@@ -6318,7 +6321,7 @@
         <v>99</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>541</v>
@@ -6472,7 +6475,7 @@
         <v>470</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>234</v>
@@ -6504,7 +6507,7 @@
         <v>470</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>548</v>
@@ -6888,7 +6891,7 @@
         <v>524</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>536</v>
@@ -6917,7 +6920,7 @@
         <v>524</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>533</v>
@@ -6955,7 +6958,7 @@
         <v>241</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>245</v>
@@ -6972,7 +6975,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>176</v>
@@ -6989,7 +6992,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>554</v>
@@ -7006,7 +7009,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>555</v>
@@ -7023,7 +7026,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>556</v>
@@ -7040,7 +7043,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>557</v>
@@ -7057,7 +7060,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>558</v>
@@ -7074,7 +7077,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>177</v>
@@ -7091,7 +7094,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>562</v>
@@ -7108,7 +7111,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>561</v>
@@ -7125,7 +7128,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>560</v>
@@ -7142,7 +7145,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>559</v>
@@ -7159,7 +7162,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>544</v>
@@ -7176,7 +7179,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>179</v>
@@ -7193,7 +7196,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>532</v>
@@ -7210,7 +7213,7 @@
         <v>528</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>515</v>
@@ -7223,7 +7226,7 @@
         <v>511</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>176</v>
@@ -7236,7 +7239,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>180</v>
@@ -7253,7 +7256,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>181</v>
@@ -7270,7 +7273,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>182</v>
@@ -7287,7 +7290,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>183</v>
@@ -7304,7 +7307,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>184</v>
@@ -7321,7 +7324,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>176</v>
@@ -7338,7 +7341,7 @@
         <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>185</v>
@@ -7355,7 +7358,7 @@
         <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>186</v>
@@ -7372,7 +7375,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>187</v>
@@ -7389,7 +7392,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>188</v>
@@ -7423,7 +7426,7 @@
         <v>50</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>190</v>
@@ -7440,7 +7443,7 @@
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>247</v>
@@ -7457,7 +7460,7 @@
         <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>246</v>
@@ -7474,7 +7477,7 @@
         <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>191</v>
@@ -7491,7 +7494,7 @@
         <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>192</v>
@@ -7508,7 +7511,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>182</v>
@@ -7525,7 +7528,7 @@
         <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>193</v>
@@ -7542,7 +7545,7 @@
         <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>194</v>
@@ -7559,7 +7562,7 @@
         <v>64</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>195</v>
@@ -7576,7 +7579,7 @@
         <v>66</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>196</v>
@@ -7593,7 +7596,7 @@
         <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>197</v>
@@ -7610,7 +7613,7 @@
         <v>545</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>198</v>
@@ -7627,7 +7630,7 @@
         <v>71</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>199</v>
@@ -7644,7 +7647,7 @@
         <v>73</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>200</v>
@@ -7661,7 +7664,7 @@
         <v>75</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>201</v>
@@ -7678,7 +7681,7 @@
         <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>202</v>
@@ -7695,7 +7698,7 @@
         <v>79</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>203</v>
@@ -7712,7 +7715,7 @@
         <v>81</v>
       </c>
       <c r="B46" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>204</v>
@@ -7729,7 +7732,7 @@
         <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>205</v>
@@ -7746,7 +7749,7 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>206</v>
@@ -7763,7 +7766,7 @@
         <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>207</v>
@@ -7780,7 +7783,7 @@
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>208</v>
@@ -7797,7 +7800,7 @@
         <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>209</v>
@@ -7814,7 +7817,7 @@
         <v>93</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>210</v>
@@ -7831,7 +7834,7 @@
         <v>95</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>211</v>
@@ -7848,7 +7851,7 @@
         <v>97</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>212</v>
@@ -7865,7 +7868,7 @@
         <v>100</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>213</v>
@@ -7882,7 +7885,7 @@
         <v>102</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>214</v>
@@ -7899,7 +7902,7 @@
         <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>201</v>
@@ -7916,7 +7919,7 @@
         <v>105</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>215</v>
@@ -7933,7 +7936,7 @@
         <v>107</v>
       </c>
       <c r="B59" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>216</v>
@@ -7950,7 +7953,7 @@
         <v>109</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>217</v>
@@ -7967,7 +7970,7 @@
         <v>111</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>531</v>
@@ -7982,7 +7985,7 @@
         <v>113</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>218</v>
@@ -7999,7 +8002,7 @@
         <v>115</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>200</v>
@@ -8016,7 +8019,7 @@
         <v>116</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>178</v>
@@ -8031,7 +8034,7 @@
         <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>219</v>
@@ -8046,7 +8049,7 @@
         <v>119</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>220</v>
@@ -8063,7 +8066,7 @@
         <v>121</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>221</v>
@@ -8080,7 +8083,7 @@
         <v>123</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>222</v>
@@ -8097,7 +8100,7 @@
         <v>125</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>223</v>
@@ -8114,7 +8117,7 @@
         <v>127</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>224</v>
@@ -8131,7 +8134,7 @@
         <v>129</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>225</v>
@@ -8148,7 +8151,7 @@
         <v>131</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>226</v>
@@ -8165,7 +8168,7 @@
         <v>133</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>227</v>
@@ -8182,7 +8185,7 @@
         <v>135</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>228</v>
@@ -8199,7 +8202,7 @@
         <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>229</v>
@@ -8214,7 +8217,7 @@
         <v>139</v>
       </c>
       <c r="B76" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>230</v>
@@ -8231,7 +8234,7 @@
         <v>141</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>231</v>
@@ -8248,7 +8251,7 @@
         <v>542</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>43</v>
@@ -8261,7 +8264,7 @@
         <v>517</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>518</v>
@@ -8278,7 +8281,7 @@
         <v>538</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>540</v>
@@ -8291,7 +8294,7 @@
         <v>539</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>541</v>
@@ -8318,7 +8321,7 @@
         <v>146</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>232</v>
@@ -8335,7 +8338,7 @@
         <v>148</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>549</v>
@@ -8352,7 +8355,7 @@
         <v>150</v>
       </c>
       <c r="B85" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>233</v>
@@ -8369,7 +8372,7 @@
         <v>152</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>234</v>
@@ -8386,7 +8389,7 @@
         <v>154</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>548</v>
@@ -8403,7 +8406,7 @@
         <v>156</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>235</v>
@@ -8420,7 +8423,7 @@
         <v>158</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>546</v>
@@ -8437,7 +8440,7 @@
         <v>160</v>
       </c>
       <c r="B90" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>236</v>
@@ -8454,7 +8457,7 @@
         <v>162</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>237</v>
@@ -8471,7 +8474,7 @@
         <v>163</v>
       </c>
       <c r="B92" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>547</v>
@@ -8488,7 +8491,7 @@
         <v>165</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>543</v>
@@ -8505,7 +8508,7 @@
         <v>167</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>224</v>
@@ -8522,7 +8525,7 @@
         <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>521</v>
@@ -8539,7 +8542,7 @@
         <v>170</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>238</v>
@@ -8556,7 +8559,7 @@
         <v>172</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>239</v>
@@ -8573,7 +8576,7 @@
         <v>174</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>240</v>
@@ -8590,7 +8593,7 @@
         <v>523</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>536</v>
@@ -8607,7 +8610,7 @@
         <v>529</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>533</v>

</xml_diff>